<commit_message>
Lecture 5.0 Video Links
Lecture 5.0 Video Links
</commit_message>
<xml_diff>
--- a/Schedule/schedule.xlsx
+++ b/Schedule/schedule.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://indiana-my.sharepoint.com/personal/dlovele_iu_edu/Documents/Courses/ENGR-E-399-599-VLSI/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dlovele/Documents/GitHub/iu-vlsi/Schedule/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="103" documentId="8_{60A5E32C-5E48-8840-898C-900DC1358B8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E63A4ABA-4D50-4942-A23E-B70EC5E51F86}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{31944614-81E2-C445-A2A9-39C8D24F9558}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="18400" yWindow="3380" windowWidth="28040" windowHeight="17440" xr2:uid="{B06FCACC-7A90-6240-A88B-5F618B4AAD7E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
   <si>
     <t>Date</t>
   </si>
@@ -86,12 +86,6 @@
     <t>Lab 1</t>
   </si>
   <si>
-    <t>2.0 - Circuits and Layout Part 1</t>
-  </si>
-  <si>
-    <t>2.0 - Circuits and Layout Part 2</t>
-  </si>
-  <si>
     <t>3.0 - CMOS Transistor Theory</t>
   </si>
   <si>
@@ -120,6 +114,15 @@
   </si>
   <si>
     <t>5.0 - DC and Transient Analysis</t>
+  </si>
+  <si>
+    <t>2.1 - Circuits and Layout Part 1</t>
+  </si>
+  <si>
+    <t>2.2 - Circuits and Layout Part 2</t>
+  </si>
+  <si>
+    <t>https://iu.zoom.us/rec/share/Xubuchvq8ycmR_WQz2GwuMwlpqEnvuU-Nph_SxxNFBwEU1oLzMLGcA_NrpX54rg.UX0vVf-SQbjjsG-A</t>
   </si>
 </sst>
 </file>
@@ -529,7 +532,7 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -597,7 +600,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="D3" s="5">
         <v>2.1</v>
@@ -619,7 +622,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="D4" s="5">
         <v>2.2000000000000002</v>
@@ -646,7 +649,7 @@
       <c r="F5" s="5"/>
       <c r="G5" s="5"/>
       <c r="H5" s="7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -657,7 +660,7 @@
         <v>5</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D6" s="5">
         <v>3</v>
@@ -665,7 +668,7 @@
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
       <c r="H6" s="7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
@@ -676,7 +679,7 @@
         <v>6</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D7" s="5">
         <v>4.0999999999999996</v>
@@ -685,7 +688,7 @@
         <v>9</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
@@ -696,16 +699,16 @@
         <v>7</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D8" s="5">
         <v>4.2</v>
       </c>
       <c r="G8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="H8" s="8" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
@@ -716,10 +719,13 @@
         <v>8</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E9" t="s">
         <v>14</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
@@ -732,9 +738,6 @@
       <c r="E10" t="s">
         <v>15</v>
       </c>
-      <c r="G10" t="s">
-        <v>14</v>
-      </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
@@ -744,7 +747,7 @@
         <v>10</v>
       </c>
       <c r="G11" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
@@ -755,7 +758,7 @@
         <v>11</v>
       </c>
       <c r="G12" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
@@ -764,6 +767,9 @@
       </c>
       <c r="B13" s="4">
         <v>12</v>
+      </c>
+      <c r="G13" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
@@ -790,6 +796,7 @@
     <hyperlink ref="H6" r:id="rId4" xr:uid="{7FE0B1B5-30FD-6F4E-ABAA-60688F77715F}"/>
     <hyperlink ref="H5" r:id="rId5" xr:uid="{E22AF520-BC7E-1744-BF40-84716A8AC000}"/>
     <hyperlink ref="H8" r:id="rId6" xr:uid="{499CD6A5-BCD1-0346-B2EF-ABD92106182B}"/>
+    <hyperlink ref="H9" r:id="rId7" xr:uid="{EC97833A-6646-D74E-B116-F85496FD895A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Schedule and Video Link Update
Update to schedule and Zoom videos following 2/6 lecture
</commit_message>
<xml_diff>
--- a/Schedule/schedule.xlsx
+++ b/Schedule/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dlovele/Documents/GitHub/iu-vlsi/Schedule/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{31944614-81E2-C445-A2A9-39C8D24F9558}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{601DF1BA-C751-5F4E-9AE5-D6232376B9A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="18400" yWindow="3380" windowWidth="28040" windowHeight="17440" xr2:uid="{B06FCACC-7A90-6240-A88B-5F618B4AAD7E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="32">
   <si>
     <t>Date</t>
   </si>
@@ -89,9 +89,6 @@
     <t>3.0 - CMOS Transistor Theory</t>
   </si>
   <si>
-    <t>Quiz 1</t>
-  </si>
-  <si>
     <t>https://iu.zoom.us/rec/share/d0ZI9uRriuLMvON9qcujOuFFerdCgZnD6vthvu2jYytd7UnpaZZcXpkZFFXbLB01.SWT6K2Cm76BQzTH7</t>
   </si>
   <si>
@@ -123,6 +120,18 @@
   </si>
   <si>
     <t>https://iu.zoom.us/rec/share/Xubuchvq8ycmR_WQz2GwuMwlpqEnvuU-Nph_SxxNFBwEU1oLzMLGcA_NrpX54rg.UX0vVf-SQbjjsG-A</t>
+  </si>
+  <si>
+    <t>Tutorial - Gate Optimization and Buffer Design</t>
+  </si>
+  <si>
+    <t>https://iu.zoom.us/rec/share/TAu5wQAkgguM92x84qoZu5pTdF9lLYijKJ2AXb-5RaLxx2F2u3TnhbwLHJfoRU2F.3L3P76JRY2GSMT1B?startTime=1707243575000</t>
+  </si>
+  <si>
+    <t>HW 1/Quiz 1</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
 </sst>
 </file>
@@ -538,7 +547,7 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.83203125" bestFit="1" customWidth="1"/>
@@ -600,7 +609,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D3" s="5">
         <v>2.1</v>
@@ -622,7 +631,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D4" s="5">
         <v>2.2000000000000002</v>
@@ -644,12 +653,14 @@
       <c r="C5" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="5"/>
+      <c r="D5" s="5" t="s">
+        <v>31</v>
+      </c>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
       <c r="G5" s="5"/>
       <c r="H5" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -668,7 +679,7 @@
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
       <c r="H6" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
@@ -679,7 +690,7 @@
         <v>6</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D7" s="5">
         <v>4.0999999999999996</v>
@@ -688,7 +699,7 @@
         <v>9</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
@@ -699,16 +710,16 @@
         <v>7</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D8" s="5">
         <v>4.2</v>
       </c>
       <c r="G8" t="s">
+        <v>20</v>
+      </c>
+      <c r="H8" s="8" t="s">
         <v>21</v>
-      </c>
-      <c r="H8" s="8" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
@@ -719,13 +730,13 @@
         <v>8</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="E9" t="s">
-        <v>14</v>
+        <v>24</v>
+      </c>
+      <c r="D9" s="5">
+        <v>5</v>
       </c>
       <c r="H9" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
@@ -735,8 +746,17 @@
       <c r="B10" s="4">
         <v>9</v>
       </c>
+      <c r="C10" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>31</v>
+      </c>
       <c r="E10" t="s">
-        <v>15</v>
+        <v>14</v>
+      </c>
+      <c r="H10" s="8" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
@@ -746,8 +766,8 @@
       <c r="B11" s="4">
         <v>10</v>
       </c>
-      <c r="G11" t="s">
-        <v>14</v>
+      <c r="E11" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
@@ -758,7 +778,7 @@
         <v>11</v>
       </c>
       <c r="G12" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
@@ -797,6 +817,7 @@
     <hyperlink ref="H5" r:id="rId5" xr:uid="{E22AF520-BC7E-1744-BF40-84716A8AC000}"/>
     <hyperlink ref="H8" r:id="rId6" xr:uid="{499CD6A5-BCD1-0346-B2EF-ABD92106182B}"/>
     <hyperlink ref="H9" r:id="rId7" xr:uid="{EC97833A-6646-D74E-B116-F85496FD895A}"/>
+    <hyperlink ref="H10" r:id="rId8" xr:uid="{68FC2FF9-4BC4-854F-8705-89DD502A2913}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Major Update -Cadence Library/Slides 7/Zoom Links
Update to IU STD CELL Lib
Slides 7.0
Zoom link + schedule update
</commit_message>
<xml_diff>
--- a/Schedule/schedule.xlsx
+++ b/Schedule/schedule.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dlovele/Documents/GitHub/iu-vlsi/Schedule/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{601DF1BA-C751-5F4E-9AE5-D6232376B9A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{884B3F3F-D23F-C840-A9A4-DF833CF33333}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="18400" yWindow="3380" windowWidth="28040" windowHeight="17440" xr2:uid="{B06FCACC-7A90-6240-A88B-5F618B4AAD7E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="38">
   <si>
     <t>Date</t>
   </si>
@@ -128,10 +128,28 @@
     <t>https://iu.zoom.us/rec/share/TAu5wQAkgguM92x84qoZu5pTdF9lLYijKJ2AXb-5RaLxx2F2u3TnhbwLHJfoRU2F.3L3P76JRY2GSMT1B?startTime=1707243575000</t>
   </si>
   <si>
-    <t>HW 1/Quiz 1</t>
-  </si>
-  <si>
     <t>NA</t>
+  </si>
+  <si>
+    <t>7.0 - Power</t>
+  </si>
+  <si>
+    <t>6.1 - Logical Effort Part 1</t>
+  </si>
+  <si>
+    <t>6.2 - Logical Effort Part 2</t>
+  </si>
+  <si>
+    <t>Lab  1</t>
+  </si>
+  <si>
+    <t>Quiz 1</t>
+  </si>
+  <si>
+    <t>https://iu.zoom.us/rec/share/IB0cyZD_eISgemVTiFcyU12VHnYR-nnvtp9ufdfrSWPA2uJRqo_G2Z5NIcCkVlR9.C4kofYzOqIlKnWWL</t>
+  </si>
+  <si>
+    <t>https://iu.zoom.us/rec/share/3GW27LneiHNfTu4meorvl4ZkINGOM493rWDRJw5Tc2lGb7ikOhb-Y3GSUW2vEk-n.Kp6h406uHpjtf0FM</t>
   </si>
 </sst>
 </file>
@@ -541,7 +559,7 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -654,7 +672,7 @@
         <v>12</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
@@ -750,7 +768,7 @@
         <v>28</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E10" t="s">
         <v>14</v>
@@ -766,8 +784,14 @@
       <c r="B11" s="4">
         <v>10</v>
       </c>
+      <c r="C11" s="5" t="s">
+        <v>32</v>
+      </c>
       <c r="E11" t="s">
         <v>15</v>
+      </c>
+      <c r="H11" s="8" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
@@ -777,8 +801,14 @@
       <c r="B12" s="4">
         <v>11</v>
       </c>
+      <c r="C12" s="5" t="s">
+        <v>33</v>
+      </c>
       <c r="G12" t="s">
-        <v>30</v>
+        <v>14</v>
+      </c>
+      <c r="H12" s="8" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
@@ -788,7 +818,10 @@
       <c r="B13" s="4">
         <v>12</v>
       </c>
-      <c r="G13" t="s">
+      <c r="C13" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E13" t="s">
         <v>15</v>
       </c>
     </row>
@@ -799,6 +832,9 @@
       <c r="B14" s="4">
         <v>13</v>
       </c>
+      <c r="G14" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
@@ -806,6 +842,9 @@
       </c>
       <c r="B15" s="4">
         <v>14</v>
+      </c>
+      <c r="G15" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -818,6 +857,8 @@
     <hyperlink ref="H8" r:id="rId6" xr:uid="{499CD6A5-BCD1-0346-B2EF-ABD92106182B}"/>
     <hyperlink ref="H9" r:id="rId7" xr:uid="{EC97833A-6646-D74E-B116-F85496FD895A}"/>
     <hyperlink ref="H10" r:id="rId8" xr:uid="{68FC2FF9-4BC4-854F-8705-89DD502A2913}"/>
+    <hyperlink ref="H11" r:id="rId9" xr:uid="{748BB8C2-FC11-134C-B011-0BF43CCDDD37}"/>
+    <hyperlink ref="H12" r:id="rId10" xr:uid="{D24BB517-0929-6B4E-9FF5-73D44EADB8F6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Schedule and Lecture Video Update
Link to 11.1 - SRAM Part 1
</commit_message>
<xml_diff>
--- a/Schedule/schedule.xlsx
+++ b/Schedule/schedule.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://indiana-my.sharepoint.com/personal/dlovele_iu_edu/Documents/Courses/ENGR-E-399-599-VLSI/S24/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dlovele/Documents/GitHub/iu-vlsi/Schedule/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="14" documentId="13_ncr:1_{72D82A02-0668-F445-BAC8-819388D28848}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7CCACAE9-0930-B74F-9CB1-814B2D22462E}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8ADFFBA-6EDC-6F4E-8246-4D625B5D4551}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="72360" yWindow="3340" windowWidth="28040" windowHeight="17440" xr2:uid="{B06FCACC-7A90-6240-A88B-5F618B4AAD7E}"/>
+    <workbookView xWindow="17280" yWindow="5040" windowWidth="28040" windowHeight="17440" xr2:uid="{B06FCACC-7A90-6240-A88B-5F618B4AAD7E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="63">
   <si>
     <t>Date</t>
   </si>
@@ -210,6 +210,21 @@
   </si>
   <si>
     <t>Lab Notebook</t>
+  </si>
+  <si>
+    <t>11.1 - SRAM Part 1</t>
+  </si>
+  <si>
+    <t>https://iu.zoom.us/rec/share/AVOyoBq7ugqQtqP7DRvrtjO0pUq7w5SAfB4FvOXIdyeRNt91uGkWkQJ1It2QrQ9_.nFwcWDkTxE_rxWaj?startTime=1712078074000</t>
+  </si>
+  <si>
+    <t>11.2 - SRAM Part 2 + Final Project Work Day 2</t>
+  </si>
+  <si>
+    <t>Lab Notebook Part 1</t>
+  </si>
+  <si>
+    <t>HW 2</t>
   </si>
 </sst>
 </file>
@@ -622,10 +637,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE0BEA82-A198-C647-847D-48FD57D34800}">
-  <dimension ref="A1:H23"/>
+  <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -635,7 +650,7 @@
     <col min="4" max="4" width="6.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="133.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1084,6 +1099,43 @@
       </c>
       <c r="H23" t="s">
         <v>30</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24" s="2">
+        <v>45384</v>
+      </c>
+      <c r="B24" s="4">
+        <v>23</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D24">
+        <v>11</v>
+      </c>
+      <c r="H24" s="8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A25" s="2">
+        <v>45386</v>
+      </c>
+      <c r="B25" s="4">
+        <v>24</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D25">
+        <v>11</v>
+      </c>
+      <c r="E25" t="s">
+        <v>62</v>
+      </c>
+      <c r="G25" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -1106,6 +1158,7 @@
     <hyperlink ref="H20" r:id="rId16" xr:uid="{66E5D868-9E08-1C4F-AB99-58A75F28048C}"/>
     <hyperlink ref="H21" r:id="rId17" xr:uid="{C59E4932-9747-044C-9DA2-A3A79E125198}"/>
     <hyperlink ref="H22" r:id="rId18" xr:uid="{394D0932-0461-054B-8C63-FDCC6D614792}"/>
+    <hyperlink ref="H24" r:id="rId19" xr:uid="{ADCF3CFB-25AA-9A44-88D1-FBA53C400F7C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Schedule and video update
</commit_message>
<xml_diff>
--- a/Schedule/schedule.xlsx
+++ b/Schedule/schedule.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dlovele/Documents/GitHub/iu-vlsi/Schedule/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8ADFFBA-6EDC-6F4E-8246-4D625B5D4551}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75167C9A-6D82-1644-A66C-13EB2CB182F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17280" yWindow="5040" windowWidth="28040" windowHeight="17440" xr2:uid="{B06FCACC-7A90-6240-A88B-5F618B4AAD7E}"/>
+    <workbookView xWindow="22940" yWindow="7920" windowWidth="28040" windowHeight="17440" xr2:uid="{B06FCACC-7A90-6240-A88B-5F618B4AAD7E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="66">
   <si>
     <t>Date</t>
   </si>
@@ -224,7 +224,16 @@
     <t>Lab Notebook Part 1</t>
   </si>
   <si>
-    <t>HW 2</t>
+    <t>12.1 - Clocking</t>
+  </si>
+  <si>
+    <t>https://iu.zoom.us/rec/share/r40LjSsDuljX-ADcPdAabvBnSKCeUdVrQodbCKYzzWYz52RUyh2j7RLCF__uBrEB.2FuwHK_E1shbLXcE</t>
+  </si>
+  <si>
+    <t>12.2 - Clocking + Final Project Work Day 3</t>
+  </si>
+  <si>
+    <t>Final Project Work Day 4</t>
   </si>
 </sst>
 </file>
@@ -637,10 +646,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE0BEA82-A198-C647-847D-48FD57D34800}">
-  <dimension ref="A1:H25"/>
+  <dimension ref="A1:H30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1131,10 +1140,59 @@
       <c r="D25">
         <v>11</v>
       </c>
-      <c r="E25" t="s">
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B26" s="4">
+        <v>25</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D26" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B27" s="4">
+        <v>26</v>
+      </c>
+      <c r="C27" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="G25" t="s">
+      <c r="D27">
+        <v>12</v>
+      </c>
+      <c r="H27" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B28" s="4">
+        <v>27</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D28">
+        <v>12</v>
+      </c>
+      <c r="H28" s="8" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B29" s="4">
+        <v>28</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B30" s="4">
+        <v>29</v>
+      </c>
+      <c r="G30" t="s">
         <v>61</v>
       </c>
     </row>
@@ -1159,6 +1217,7 @@
     <hyperlink ref="H21" r:id="rId17" xr:uid="{C59E4932-9747-044C-9DA2-A3A79E125198}"/>
     <hyperlink ref="H22" r:id="rId18" xr:uid="{394D0932-0461-054B-8C63-FDCC6D614792}"/>
     <hyperlink ref="H24" r:id="rId19" xr:uid="{ADCF3CFB-25AA-9A44-88D1-FBA53C400F7C}"/>
+    <hyperlink ref="H28" r:id="rId20" xr:uid="{30F2F42D-D22E-AD4C-8BE7-C2E4684A8938}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>